<commit_message>
fix download file error
</commit_message>
<xml_diff>
--- a/src/main/java/com/backend/file/error-file-voucher.xlsx
+++ b/src/main/java/com/backend/file/error-file-voucher.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Quanghui</t>
+  </si>
+  <si>
+    <t>Thành Test nè</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +405,44 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -674,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,6 +752,22 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyBorder="true" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyBorder="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,7 +1130,7 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="14">
+      <c r="I1" t="s" s="22">
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1082,19 +1139,19 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="16">
+      <c r="A2" t="n" s="24">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s" s="16">
-        <v>18</v>
-      </c>
-      <c r="F2" t="n" s="16">
+      <c r="C2" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="F2" t="n" s="24">
         <v>0.0</v>
       </c>
-      <c r="K2" t="s" s="15">
+      <c r="K2" t="s" s="23">
         <v>16</v>
       </c>
     </row>

</xml_diff>